<commit_message>
massive refactor to put VARS into special sections
</commit_message>
<xml_diff>
--- a/balance.xlsx
+++ b/balance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="electrical" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="324">
   <si>
     <t>W/m2</t>
   </si>
@@ -926,6 +926,81 @@
   </si>
   <si>
     <t>http://www.quallion.com/sub-sp-ql075ka.asp</t>
+  </si>
+  <si>
+    <t>1Mm</t>
+  </si>
+  <si>
+    <t>4Mm</t>
+  </si>
+  <si>
+    <t>8Mm</t>
+  </si>
+  <si>
+    <t>16Mm</t>
+  </si>
+  <si>
+    <t>250Mm</t>
+  </si>
+  <si>
+    <t>10Gm</t>
+  </si>
+  <si>
+    <t>65Gm</t>
+  </si>
+  <si>
+    <t>575Gm</t>
+  </si>
+  <si>
+    <t>using…</t>
+  </si>
+  <si>
+    <t>Molniya</t>
+  </si>
+  <si>
+    <t>dist Mm</t>
+  </si>
+  <si>
+    <t>satellite</t>
+  </si>
+  <si>
+    <t>L4/L5</t>
+  </si>
+  <si>
+    <t>Deep</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>omni</t>
+  </si>
+  <si>
+    <t>comms</t>
+  </si>
+  <si>
+    <t>dish1</t>
+  </si>
+  <si>
+    <t>dish2</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>XXL</t>
+  </si>
+  <si>
+    <t>needed</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1062,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -997,12 +1072,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1020,25 +1089,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1062,7 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1082,22 +1133,22 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1124,28 +1175,16 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1169,22 +1208,22 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1193,13 +1232,13 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1611,11 +1650,11 @@
       <c r="J5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="24">
         <f>D8</f>
         <v>6.9444444444444448E-2</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="24">
         <f>N3*3600</f>
         <v>6408</v>
       </c>
@@ -1794,7 +1833,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D15" s="36">
+      <c r="D15" s="32">
         <f>600000</f>
         <v>600000</v>
       </c>
@@ -1832,7 +1871,7 @@
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="36">
+      <c r="D17" s="32">
         <v>2868750</v>
       </c>
       <c r="E17" s="1">
@@ -1849,7 +1888,7 @@
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="37">
+      <c r="D19" s="33">
         <v>3531600000000</v>
       </c>
       <c r="E19" s="19">
@@ -1858,7 +1897,7 @@
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="36" t="s">
         <v>129</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -1866,7 +1905,7 @@
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="36" t="s">
         <v>130</v>
       </c>
       <c r="E21" s="19">
@@ -1875,7 +1914,7 @@
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="26">
+      <c r="D22" s="23">
         <f>E21/E23*E19</f>
         <v>1195.2859282940951</v>
       </c>
@@ -1884,7 +1923,7 @@
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="36" t="s">
         <v>131</v>
       </c>
       <c r="E23" s="19">
@@ -1898,7 +1937,7 @@
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="41">
+      <c r="D25" s="37">
         <v>0.19</v>
       </c>
     </row>
@@ -1979,11 +2018,11 @@
         <f>E2/3600</f>
         <v>0.20000000000000004</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="36">
         <f>A2*B2*C2*1*0.03</f>
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="H2" s="46">
+      <c r="H2" s="42">
         <f>G2*1.25</f>
         <v>0.10800000000000001</v>
       </c>
@@ -2025,7 +2064,7 @@
       <c r="F1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="43" t="s">
         <v>293</v>
       </c>
     </row>
@@ -2044,7 +2083,7 @@
         <f>PI()*C2^2*B2</f>
         <v>0.25464081078901646</v>
       </c>
-      <c r="E2" s="46">
+      <c r="E2" s="42">
         <f>D2*2.4</f>
         <v>0.61113794589363946</v>
       </c>
@@ -2074,7 +2113,7 @@
         <f>PI()*C3^2*B3</f>
         <v>1.2271846303085129E-2</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="42">
         <f>D3*2.1</f>
         <v>2.5770877236478772E-2</v>
       </c>
@@ -2151,7 +2190,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K12" s="47" t="s">
+      <c r="K12" s="43" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2298,42 +2337,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="T1" s="48" t="s">
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="T1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AB1" s="48" t="s">
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AB1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AJ1" s="48" t="s">
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AJ1" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="48"/>
+      <c r="AK1" s="44"/>
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
     </row>
     <row r="2" spans="1:47" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F2" s="13" t="s">
@@ -2552,7 +2591,7 @@
       <c r="AR3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AS3" s="41">
+      <c r="AS3" s="37">
         <v>12.815</v>
       </c>
     </row>
@@ -2675,7 +2714,7 @@
       <c r="AR4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AS4" s="41">
+      <c r="AS4" s="37">
         <v>1.5</v>
       </c>
       <c r="AT4" s="1" t="s">
@@ -2921,7 +2960,7 @@
       <c r="AR6" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="AS6" s="41">
+      <c r="AS6" s="37">
         <v>230</v>
       </c>
       <c r="AT6" s="1">
@@ -2956,11 +2995,11 @@
       </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="E9" s="38"/>
+      <c r="E9" s="34"/>
       <c r="AR9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AS9" s="41">
+      <c r="AS9" s="37">
         <v>25</v>
       </c>
     </row>
@@ -2974,17 +3013,17 @@
       <c r="C10" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="38" t="str">
+      <c r="E10" s="34" t="str">
         <f>IF(D10="--n/a--","",IF(C10="Hyperg","Hypergolic",C10))&amp;"-"</f>
         <v>-</v>
       </c>
       <c r="AR10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AS10" s="41">
+      <c r="AS10" s="37">
         <v>1.5</v>
       </c>
       <c r="AT10" s="1" t="s">
@@ -3005,10 +3044,10 @@
       <c r="C11" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E11" s="38" t="str">
+      <c r="E11" s="34" t="str">
         <f t="shared" ref="E11:E74" si="1">IF(D11="--n/a--","",IF(C11="Hyperg","Hypergolic",C11))&amp;"-"</f>
         <v>-</v>
       </c>
@@ -3033,14 +3072,14 @@
       <c r="D12" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="38" t="str">
+      <c r="E12" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
       <c r="AR12" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="AS12" s="41">
+      <c r="AS12" s="37">
         <v>230</v>
       </c>
       <c r="AT12" s="1">
@@ -3061,7 +3100,7 @@
       <c r="D13" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="38" t="str">
+      <c r="E13" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3083,10 +3122,10 @@
       <c r="C14" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="38" t="str">
+      <c r="E14" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3101,10 +3140,10 @@
       <c r="C15" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E15" s="38" t="str">
+      <c r="E15" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3122,7 +3161,7 @@
       <c r="D16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="38" t="str">
+      <c r="E16" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3140,7 +3179,7 @@
       <c r="D17" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E17" s="38" t="str">
+      <c r="E17" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3155,10 +3194,10 @@
       <c r="C18" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E18" s="38" t="str">
+      <c r="E18" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3173,10 +3212,10 @@
       <c r="C19" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="38" t="str">
+      <c r="E19" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3194,7 +3233,7 @@
       <c r="D20" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E20" s="38" t="str">
+      <c r="E20" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3212,7 +3251,7 @@
       <c r="D21" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E21" s="38" t="str">
+      <c r="E21" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3227,10 +3266,10 @@
       <c r="C22" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E22" s="38" t="str">
+      <c r="E22" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3245,10 +3284,10 @@
       <c r="C23" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E23" s="38" t="str">
+      <c r="E23" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3266,7 +3305,7 @@
       <c r="D24" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="38" t="str">
+      <c r="E24" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3285,7 +3324,7 @@
       <c r="D25" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E25" s="38" t="str">
+      <c r="E25" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3303,7 +3342,7 @@
       <c r="D26" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="38" t="str">
+      <c r="E26" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3321,7 +3360,7 @@
       <c r="D27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E27" s="38" t="str">
+      <c r="E27" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3339,7 +3378,7 @@
       <c r="D28" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E28" s="38" t="str">
+      <c r="E28" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3357,7 +3396,7 @@
       <c r="D29" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E29" s="38" t="str">
+      <c r="E29" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3375,7 +3414,7 @@
       <c r="D30" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E30" s="38" t="str">
+      <c r="E30" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3393,7 +3432,7 @@
       <c r="D31" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="38" t="str">
+      <c r="E31" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3411,7 +3450,7 @@
       <c r="D32" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E32" s="38" t="str">
+      <c r="E32" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3429,7 +3468,7 @@
       <c r="D33" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E33" s="38" t="str">
+      <c r="E33" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3447,7 +3486,7 @@
       <c r="D34" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E34" s="38" t="str">
+      <c r="E34" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3465,7 +3504,7 @@
       <c r="D35" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E35" s="38" t="str">
+      <c r="E35" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3483,7 +3522,7 @@
       <c r="D36" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E36" s="38" t="str">
+      <c r="E36" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3501,7 +3540,7 @@
       <c r="D37" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E37" s="38" t="str">
+      <c r="E37" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3519,7 +3558,7 @@
       <c r="D38" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E38" s="38" t="str">
+      <c r="E38" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3537,7 +3576,7 @@
       <c r="D39" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E39" s="38" t="str">
+      <c r="E39" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3555,7 +3594,7 @@
       <c r="D40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E40" s="38" t="str">
+      <c r="E40" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3573,7 +3612,7 @@
       <c r="D41" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="38" t="str">
+      <c r="E41" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydraz-</v>
       </c>
@@ -3591,7 +3630,7 @@
       <c r="D42" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E42" s="38" t="str">
+      <c r="E42" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3609,7 +3648,7 @@
       <c r="D43" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E43" s="38" t="str">
+      <c r="E43" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3627,11 +3666,11 @@
       <c r="D44" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="38" t="str">
+      <c r="E44" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
-      <c r="O44" s="43"/>
+      <c r="O44" s="39"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -3643,10 +3682,10 @@
       <c r="C45" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="38" t="s">
+      <c r="D45" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E45" s="38" t="str">
+      <c r="E45" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3664,7 +3703,7 @@
       <c r="D46" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E46" s="38" t="str">
+      <c r="E46" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3682,7 +3721,7 @@
       <c r="D47" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E47" s="38" t="str">
+      <c r="E47" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3700,7 +3739,7 @@
       <c r="D48" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E48" s="38" t="str">
+      <c r="E48" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3715,10 +3754,10 @@
       <c r="C49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D49" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E49" s="38" t="str">
+      <c r="E49" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3736,7 +3775,7 @@
       <c r="D50" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E50" s="38" t="str">
+      <c r="E50" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3754,7 +3793,7 @@
       <c r="D51" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E51" s="38" t="str">
+      <c r="E51" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3772,7 +3811,7 @@
       <c r="D52" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E52" s="38" t="str">
+      <c r="E52" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hypergolic-</v>
       </c>
@@ -3787,10 +3826,10 @@
       <c r="C53" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D53" s="38" t="s">
+      <c r="D53" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E53" s="38" t="str">
+      <c r="E53" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3808,7 +3847,7 @@
       <c r="D54" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="38" t="str">
+      <c r="E54" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3826,7 +3865,7 @@
       <c r="D55" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E55" s="38" t="str">
+      <c r="E55" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3841,10 +3880,10 @@
       <c r="C56" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D56" s="38" t="s">
+      <c r="D56" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E56" s="38" t="str">
+      <c r="E56" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3859,10 +3898,10 @@
       <c r="C57" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D57" s="38" t="s">
+      <c r="D57" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E57" s="38" t="str">
+      <c r="E57" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3880,7 +3919,7 @@
       <c r="D58" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E58" s="38" t="str">
+      <c r="E58" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3898,7 +3937,7 @@
       <c r="D59" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E59" s="38" t="str">
+      <c r="E59" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3913,10 +3952,10 @@
       <c r="C60" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D60" s="38" t="s">
+      <c r="D60" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E60" s="38" t="str">
+      <c r="E60" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3931,10 +3970,10 @@
       <c r="C61" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D61" s="38" t="s">
+      <c r="D61" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E61" s="38" t="str">
+      <c r="E61" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -3952,7 +3991,7 @@
       <c r="D62" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E62" s="38" t="str">
+      <c r="E62" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -3970,7 +4009,7 @@
       <c r="D63" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E63" s="38" t="str">
+      <c r="E63" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -3985,10 +4024,10 @@
       <c r="C64" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D64" s="38" t="s">
+      <c r="D64" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E64" s="38" t="str">
+      <c r="E64" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -4003,10 +4042,10 @@
       <c r="C65" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D65" s="38" t="s">
+      <c r="D65" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E65" s="38" t="str">
+      <c r="E65" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -4024,7 +4063,7 @@
       <c r="D66" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E66" s="38" t="str">
+      <c r="E66" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -4042,7 +4081,7 @@
       <c r="D67" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E67" s="38" t="str">
+      <c r="E67" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -4057,10 +4096,10 @@
       <c r="C68" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D68" s="38" t="s">
+      <c r="D68" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E68" s="38" t="str">
+      <c r="E68" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -4075,10 +4114,10 @@
       <c r="C69" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D69" s="38" t="s">
+      <c r="D69" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E69" s="38" t="str">
+      <c r="E69" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -4096,7 +4135,7 @@
       <c r="D70" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E70" s="38" t="str">
+      <c r="E70" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -4114,7 +4153,7 @@
       <c r="D71" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E71" s="38" t="str">
+      <c r="E71" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Kerolox-</v>
       </c>
@@ -4129,10 +4168,10 @@
       <c r="C72" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D72" s="38" t="s">
+      <c r="D72" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E72" s="38" t="str">
+      <c r="E72" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -4147,10 +4186,10 @@
       <c r="C73" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D73" s="38" t="s">
+      <c r="D73" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E73" s="38" t="str">
+      <c r="E73" s="34" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
@@ -4168,7 +4207,7 @@
       <c r="D74" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E74" s="38" t="str">
+      <c r="E74" s="34" t="str">
         <f t="shared" si="1"/>
         <v>Hydrolox-</v>
       </c>
@@ -4186,7 +4225,7 @@
       <c r="D75" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E75" s="38" t="str">
+      <c r="E75" s="34" t="str">
         <f t="shared" ref="E75:E105" si="2">IF(D75="--n/a--","",IF(C75="Hyperg","Hypergolic",C75))&amp;"-"</f>
         <v>Kerolox-</v>
       </c>
@@ -4201,10 +4240,10 @@
       <c r="C76" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D76" s="38" t="s">
+      <c r="D76" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E76" s="38" t="str">
+      <c r="E76" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4219,10 +4258,10 @@
       <c r="C77" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D77" s="38" t="s">
+      <c r="D77" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E77" s="38" t="str">
+      <c r="E77" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4240,7 +4279,7 @@
       <c r="D78" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E78" s="38" t="str">
+      <c r="E78" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Hydrolox-</v>
       </c>
@@ -4258,7 +4297,7 @@
       <c r="D79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E79" s="38" t="str">
+      <c r="E79" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Kerolox-</v>
       </c>
@@ -4273,10 +4312,10 @@
       <c r="C80" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D80" s="38" t="s">
+      <c r="D80" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E80" s="38" t="str">
+      <c r="E80" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4291,10 +4330,10 @@
       <c r="C81" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D81" s="38" t="s">
+      <c r="D81" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E81" s="38" t="str">
+      <c r="E81" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4312,7 +4351,7 @@
       <c r="D82" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E82" s="38" t="str">
+      <c r="E82" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Hydrolox-</v>
       </c>
@@ -4330,7 +4369,7 @@
       <c r="D83" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E83" s="38" t="str">
+      <c r="E83" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Kerolox-</v>
       </c>
@@ -4345,10 +4384,10 @@
       <c r="C84" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D84" s="38" t="s">
+      <c r="D84" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E84" s="38" t="str">
+      <c r="E84" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4363,10 +4402,10 @@
       <c r="C85" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D85" s="38" t="s">
+      <c r="D85" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E85" s="38" t="str">
+      <c r="E85" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4384,7 +4423,7 @@
       <c r="D86" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E86" s="38" t="str">
+      <c r="E86" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Hydrolox-</v>
       </c>
@@ -4402,7 +4441,7 @@
       <c r="D87" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E87" s="38" t="str">
+      <c r="E87" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Kerolox-</v>
       </c>
@@ -4417,10 +4456,10 @@
       <c r="C88" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D88" s="38" t="s">
+      <c r="D88" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E88" s="38" t="str">
+      <c r="E88" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4435,10 +4474,10 @@
       <c r="C89" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D89" s="38" t="s">
+      <c r="D89" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E89" s="38" t="str">
+      <c r="E89" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4456,7 +4495,7 @@
       <c r="D90" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E90" s="38" t="str">
+      <c r="E90" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Hydrolox-</v>
       </c>
@@ -4474,7 +4513,7 @@
       <c r="D91" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E91" s="38" t="str">
+      <c r="E91" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Kerolox-</v>
       </c>
@@ -4489,10 +4528,10 @@
       <c r="C92" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D92" s="38" t="s">
+      <c r="D92" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E92" s="38" t="str">
+      <c r="E92" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4507,10 +4546,10 @@
       <c r="C93" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D93" s="38" t="s">
+      <c r="D93" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E93" s="38" t="str">
+      <c r="E93" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4528,7 +4567,7 @@
       <c r="D94" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E94" s="38" t="str">
+      <c r="E94" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Hydrolox-</v>
       </c>
@@ -4546,7 +4585,7 @@
       <c r="D95" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E95" s="38" t="str">
+      <c r="E95" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Kerolox-</v>
       </c>
@@ -4561,10 +4600,10 @@
       <c r="C96" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E96" s="38" t="str">
+      <c r="E96" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4579,10 +4618,10 @@
       <c r="C97" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D97" s="38" t="s">
+      <c r="D97" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E97" s="38" t="str">
+      <c r="E97" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4600,7 +4639,7 @@
       <c r="D98" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E98" s="38" t="str">
+      <c r="E98" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Hydrolox-</v>
       </c>
@@ -4618,7 +4657,7 @@
       <c r="D99" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E99" s="38" t="str">
+      <c r="E99" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Kerolox-</v>
       </c>
@@ -4633,10 +4672,10 @@
       <c r="C100" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D100" s="38" t="s">
+      <c r="D100" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E100" s="38" t="str">
+      <c r="E100" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4651,10 +4690,10 @@
       <c r="C101" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D101" s="38" t="s">
+      <c r="D101" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E101" s="38" t="str">
+      <c r="E101" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4672,7 +4711,7 @@
       <c r="D102" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E102" s="38" t="str">
+      <c r="E102" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Hydrolox-</v>
       </c>
@@ -4690,7 +4729,7 @@
       <c r="D103" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E103" s="38" t="str">
+      <c r="E103" s="34" t="str">
         <f t="shared" si="2"/>
         <v>Kerolox-</v>
       </c>
@@ -4705,10 +4744,10 @@
       <c r="C104" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D104" s="38" t="s">
+      <c r="D104" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E104" s="38" t="str">
+      <c r="E104" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4723,10 +4762,10 @@
       <c r="C105" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D105" s="38" t="s">
+      <c r="D105" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="E105" s="38" t="str">
+      <c r="E105" s="34" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
@@ -4748,34 +4787,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC36"/>
+  <dimension ref="A1:BN36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="3.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="1.28515625" style="1" customWidth="1"/>
     <col min="24" max="24" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.140625" style="1" bestFit="1" customWidth="1"/>
@@ -4790,22 +4830,34 @@
     <col min="34" max="34" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="2.85546875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="42" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="1.7109375" style="1" customWidth="1"/>
-    <col min="49" max="49" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.140625" style="1"/>
+    <col min="49" max="49" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.140625" style="1"/>
+    <col min="56" max="56" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="62" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="65" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>59</v>
       </c>
@@ -4899,57 +4951,63 @@
       <c r="AL1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="AM1" s="24">
+      <c r="AM1" s="22">
         <f>AL2</f>
         <v>1</v>
       </c>
-      <c r="AN1" s="24">
+      <c r="AN1" s="22">
         <f>AL3</f>
         <v>4</v>
       </c>
-      <c r="AO1" s="24">
+      <c r="AO1" s="22">
         <f>AL4</f>
-        <v>6</v>
-      </c>
-      <c r="AP1" s="24">
+        <v>8</v>
+      </c>
+      <c r="AP1" s="22">
         <f>AL5</f>
-        <v>8</v>
-      </c>
-      <c r="AQ1" s="24">
+        <v>16</v>
+      </c>
+      <c r="AQ1" s="22">
         <f>AL6</f>
         <v>250</v>
       </c>
-      <c r="AR1" s="24">
+      <c r="AR1" s="22">
         <f>AL7</f>
         <v>10000</v>
       </c>
-      <c r="AS1" s="24">
+      <c r="AS1" s="22">
         <f>AL8</f>
         <v>65000</v>
       </c>
-      <c r="AT1" s="24">
+      <c r="AT1" s="22">
         <f>AL9</f>
         <v>575000</v>
       </c>
-      <c r="AU1" s="24">
+      <c r="AU1" s="22">
         <f>AL10</f>
         <v>1000000</v>
       </c>
-      <c r="AW1" s="1"/>
+      <c r="AW1" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="AX1" s="1"/>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
-    </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD1" s="1"/>
+      <c r="BG1" s="13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -5056,7 +5114,7 @@
         <v>1</v>
       </c>
       <c r="AM2" s="16">
-        <f>MIN($AL2,AM$1)+SQRT($AL2*AM$1)</f>
+        <f>MIN(AM$12,$AW2,MIN($AL2,AM$1)+SQRT($AL2*AM$1))</f>
         <v>2</v>
       </c>
       <c r="AN2" s="16"/>
@@ -5067,24 +5125,61 @@
       <c r="AS2" s="16"/>
       <c r="AT2" s="16"/>
       <c r="AU2" s="16"/>
-      <c r="AW2" s="1" t="s">
+      <c r="AW2" s="1">
+        <f>100*AL2</f>
+        <v>100</v>
+      </c>
+      <c r="AX2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AX2" s="16">
-        <f t="shared" ref="AX2:AX7" si="2">SUM(AY2:BA2)/1000000</f>
+      <c r="AY2" s="16">
+        <f t="shared" ref="AY2:AY7" si="2">SUM(AZ2:BB2)/1000000</f>
         <v>6.9375</v>
-      </c>
-      <c r="AY2" s="16">
-        <f>600000+2868750</f>
-        <v>3468750</v>
       </c>
       <c r="AZ2" s="16">
         <f>600000+2868750</f>
         <v>3468750</v>
       </c>
-      <c r="BA2" s="16"/>
-    </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BA2" s="16">
+        <f>600000+2868750</f>
+        <v>3468750</v>
+      </c>
+      <c r="BB2" s="16"/>
+      <c r="BD2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="BF2" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="BG2" s="13">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="13">
+        <v>4</v>
+      </c>
+      <c r="BI2" s="13">
+        <v>3</v>
+      </c>
+      <c r="BJ2" s="13">
+        <v>4</v>
+      </c>
+      <c r="BK2" s="13">
+        <v>5</v>
+      </c>
+      <c r="BL2" s="13">
+        <v>6</v>
+      </c>
+      <c r="BM2" s="13">
+        <v>7</v>
+      </c>
+      <c r="BN2" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -5194,11 +5289,11 @@
         <v>4</v>
       </c>
       <c r="AM3" s="16">
-        <f t="shared" ref="AM3:AM10" si="8">MIN($AL3,AM$1)+SQRT($AL3*AM$1)</f>
+        <f t="shared" ref="AM3:AT10" si="8">MIN(AM$12,$AW3,MIN($AL3,AM$1)+SQRT($AL3*AM$1))</f>
         <v>3</v>
       </c>
-      <c r="AN3" s="26">
-        <f t="shared" ref="AN3:AN10" si="9">MIN($AL3,AN$1)+SQRT($AL3*AN$1)</f>
+      <c r="AN3" s="16">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="AO3" s="16"/>
@@ -5208,25 +5303,70 @@
       <c r="AS3" s="16"/>
       <c r="AT3" s="16"/>
       <c r="AU3" s="16"/>
-      <c r="AW3" s="1" t="s">
+      <c r="AW3" s="1">
+        <f>100*AL3</f>
+        <v>400</v>
+      </c>
+      <c r="AX3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AX3" s="16">
+      <c r="AY3" s="16">
         <f t="shared" si="2"/>
         <v>15.668749999999999</v>
       </c>
-      <c r="AY3" s="16">
+      <c r="AZ3" s="16">
         <f>600000+2868750</f>
         <v>3468750</v>
       </c>
-      <c r="AZ3" s="16">
+      <c r="BA3" s="16">
         <v>12000000</v>
       </c>
-      <c r="BA3" s="16">
+      <c r="BB3" s="16">
         <v>200000</v>
       </c>
-    </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF3" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="BG3" s="1">
+        <f>(($BF3-BG$2)^2 )/ BG$2</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="BH3" s="1">
+        <f>(($BF3-BH$2)^2 )/ BH$2</f>
+        <v>2.8899999999999997</v>
+      </c>
+      <c r="BI3" s="1">
+        <f>(($BF3-BI$2)^2 )/ BI$2</f>
+        <v>1.92</v>
+      </c>
+      <c r="BJ3" s="4">
+        <f t="shared" ref="BG3:BN7" si="9">(($BF3-BJ$2)^2 )/ BJ$2</f>
+        <v>2.8899999999999997</v>
+      </c>
+      <c r="BK3" s="4">
+        <f t="shared" si="9"/>
+        <v>3.8720000000000008</v>
+      </c>
+      <c r="BL3" s="4">
+        <f t="shared" si="9"/>
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="BM3" s="4">
+        <f t="shared" si="9"/>
+        <v>5.8514285714285723</v>
+      </c>
+      <c r="BN3" s="4">
+        <f t="shared" si="9"/>
+        <v>6.8450000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -5262,7 +5402,7 @@
         <v>45</v>
       </c>
       <c r="L4" s="16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M4" s="16">
         <v>15</v>
@@ -5278,19 +5418,19 @@
       </c>
       <c r="Q4" s="16">
         <f>(L4/L3)^2*Q3</f>
-        <v>180</v>
+        <v>320</v>
       </c>
       <c r="R4" s="17">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>320</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="6"/>
-        <v>5.0000040000000003E-2</v>
+        <v>8.8888960000000003E-2</v>
       </c>
       <c r="T4" s="5">
         <f t="shared" si="7"/>
-        <v>3.0000024000000001</v>
+        <v>5.3333376000000001</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>41</v>
@@ -5330,19 +5470,19 @@
         <v>50468750</v>
       </c>
       <c r="AL4" s="17">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AM4" s="16">
         <f t="shared" si="8"/>
-        <v>3.4494897427831779</v>
+        <v>3.8284271247461903</v>
       </c>
       <c r="AN4" s="16">
-        <f t="shared" si="9"/>
-        <v>8.8989794855663558</v>
+        <f t="shared" si="8"/>
+        <v>9.6568542494923797</v>
       </c>
       <c r="AO4" s="16">
-        <f t="shared" ref="AO4:AO10" si="10">MIN($AL4,AO$1)+SQRT($AL4*AO$1)</f>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>16</v>
       </c>
       <c r="AP4" s="16"/>
       <c r="AQ4" s="16"/>
@@ -5350,25 +5490,71 @@
       <c r="AS4" s="16"/>
       <c r="AT4" s="16"/>
       <c r="AU4" s="16"/>
-      <c r="AW4" s="1" t="s">
+      <c r="AW4" s="1">
+        <f>1000*AL4</f>
+        <v>8000</v>
+      </c>
+      <c r="AX4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AX4" s="16">
+      <c r="AY4" s="16">
         <f t="shared" si="2"/>
         <v>50.528750000000002</v>
       </c>
-      <c r="AY4" s="16">
+      <c r="AZ4" s="16">
         <f>600000+2868750</f>
         <v>3468750</v>
       </c>
-      <c r="AZ4" s="16">
+      <c r="BA4" s="16">
         <v>47000000</v>
       </c>
-      <c r="BA4" s="16">
+      <c r="BB4" s="16">
         <v>60000</v>
       </c>
-    </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BE4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF4" s="6">
+        <f>5*BF3</f>
+        <v>3</v>
+      </c>
+      <c r="BG4" s="4">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="BH4" s="1">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="BI4" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="4">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="BK4" s="4">
+        <f t="shared" si="9"/>
+        <v>0.8</v>
+      </c>
+      <c r="BL4" s="4">
+        <f t="shared" si="9"/>
+        <v>1.5</v>
+      </c>
+      <c r="BM4" s="4">
+        <f t="shared" si="9"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="BN4" s="4">
+        <f t="shared" si="9"/>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -5383,15 +5569,15 @@
       </c>
       <c r="E5" s="16">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F5" s="16">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H5" s="16">
         <v>16</v>
@@ -5404,7 +5590,7 @@
         <v>48</v>
       </c>
       <c r="L5" s="16">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M5" s="16">
         <v>10</v>
@@ -5420,63 +5606,109 @@
       </c>
       <c r="Q5" s="16">
         <f>(L5/L4)^2*Q4</f>
-        <v>320</v>
+        <v>1280</v>
       </c>
       <c r="R5" s="17">
         <f t="shared" si="5"/>
-        <v>320</v>
+        <v>1280</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="6"/>
-        <v>8.8888960000000003E-2</v>
+        <v>0.35555584000000001</v>
       </c>
       <c r="T5" s="5">
         <f t="shared" si="7"/>
-        <v>5.3333376000000001</v>
+        <v>21.3333504</v>
       </c>
       <c r="AL5" s="17">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="AM5" s="16">
         <f t="shared" si="8"/>
-        <v>3.8284271247461903</v>
+        <v>5</v>
       </c>
       <c r="AN5" s="16">
-        <f t="shared" si="9"/>
-        <v>9.6568542494923797</v>
+        <f t="shared" si="8"/>
+        <v>12</v>
       </c>
       <c r="AO5" s="16">
-        <f t="shared" si="10"/>
-        <v>12.928203230275509</v>
-      </c>
-      <c r="AP5" s="25">
-        <f t="shared" ref="AP5:AP10" si="11">MIN($AL5,AP$1)+SQRT($AL5*AP$1)</f>
-        <v>16</v>
+        <f t="shared" si="8"/>
+        <v>19.313708498984759</v>
+      </c>
+      <c r="AP5" s="16">
+        <f t="shared" si="8"/>
+        <v>32</v>
       </c>
       <c r="AQ5" s="16"/>
       <c r="AR5" s="16"/>
       <c r="AS5" s="16"/>
       <c r="AT5" s="16"/>
       <c r="AU5" s="16"/>
-      <c r="AW5" s="1" t="s">
+      <c r="AW5" s="1">
+        <f t="shared" ref="AW5:AW10" si="10">1000*AL5</f>
+        <v>16000</v>
+      </c>
+      <c r="AX5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AX5" s="16">
+      <c r="AY5" s="16">
         <f t="shared" si="2"/>
         <v>35386.498168999999</v>
       </c>
-      <c r="AY5" s="16">
+      <c r="AZ5" s="16">
         <f>600000+2868750</f>
         <v>3468750</v>
       </c>
-      <c r="AZ5" s="16">
+      <c r="BA5" s="16">
         <v>21783189163</v>
       </c>
-      <c r="BA5" s="16">
+      <c r="BB5" s="16">
         <v>13599840256</v>
       </c>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BE5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF5" s="6">
+        <f>4*BF4</f>
+        <v>12</v>
+      </c>
+      <c r="BG5" s="1">
+        <f t="shared" si="9"/>
+        <v>121</v>
+      </c>
+      <c r="BH5" s="4">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="BI5" s="4">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="BJ5" s="4">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="BK5" s="4">
+        <f t="shared" si="9"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="BL5" s="4">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="BM5" s="4">
+        <f t="shared" si="9"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="BN5" s="4">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>84</v>
       </c>
@@ -5495,11 +5727,11 @@
       </c>
       <c r="F6" s="16">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G6" s="16">
         <f t="shared" si="3"/>
-        <v>290.84271247461902</v>
+        <v>416</v>
       </c>
       <c r="H6" s="16">
         <v>90</v>
@@ -5528,19 +5760,19 @@
       </c>
       <c r="Q6" s="16">
         <f>1.5*Q5</f>
-        <v>480</v>
+        <v>1920</v>
       </c>
       <c r="R6" s="17">
         <f t="shared" si="5"/>
-        <v>480</v>
+        <v>1920</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="6"/>
-        <v>0.13333344</v>
+        <v>0.53333375999999999</v>
       </c>
       <c r="T6" s="5">
         <f t="shared" si="7"/>
-        <v>8.0000064000000002</v>
+        <v>32.000025600000001</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>9</v>
@@ -5548,49 +5780,95 @@
       <c r="AL6" s="17">
         <v>250</v>
       </c>
-      <c r="AM6" s="25">
+      <c r="AM6" s="16">
         <f t="shared" si="8"/>
         <v>16.811388300841898</v>
       </c>
       <c r="AN6" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>35.622776601683796</v>
       </c>
       <c r="AO6" s="16">
-        <f t="shared" si="10"/>
-        <v>44.729833462074168</v>
-      </c>
-      <c r="AP6" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>52.721359549995796</v>
       </c>
+      <c r="AP6" s="16">
+        <f t="shared" si="8"/>
+        <v>79.245553203367592</v>
+      </c>
       <c r="AQ6" s="16">
-        <f>MIN($AL6,AQ$1)+SQRT($AL6*AQ$1)</f>
+        <f t="shared" si="8"/>
         <v>500</v>
       </c>
       <c r="AR6" s="16"/>
       <c r="AS6" s="16"/>
       <c r="AT6" s="16"/>
       <c r="AU6" s="16"/>
-      <c r="AW6" s="1" t="s">
+      <c r="AW6" s="1">
+        <f t="shared" si="10"/>
+        <v>250000</v>
+      </c>
+      <c r="AX6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AX6" s="16">
+      <c r="AY6" s="16">
         <f t="shared" si="2"/>
         <v>85815.547393000001</v>
       </c>
-      <c r="AY6" s="16">
+      <c r="AZ6" s="16">
         <f>600000+2868750</f>
         <v>3468750</v>
       </c>
-      <c r="AZ6" s="16">
+      <c r="BA6" s="16">
         <v>72212238387</v>
       </c>
-      <c r="BA6" s="16">
+      <c r="BB6" s="16">
         <v>13599840256</v>
       </c>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF6" s="6">
+        <f>4*BF5</f>
+        <v>48</v>
+      </c>
+      <c r="BG6" s="1">
+        <f t="shared" si="9"/>
+        <v>2209</v>
+      </c>
+      <c r="BH6" s="1">
+        <f t="shared" si="9"/>
+        <v>484</v>
+      </c>
+      <c r="BI6" s="1">
+        <f t="shared" si="9"/>
+        <v>675</v>
+      </c>
+      <c r="BJ6" s="6">
+        <f t="shared" si="9"/>
+        <v>484</v>
+      </c>
+      <c r="BK6" s="6">
+        <f t="shared" si="9"/>
+        <v>369.8</v>
+      </c>
+      <c r="BL6" s="6">
+        <f t="shared" si="9"/>
+        <v>294</v>
+      </c>
+      <c r="BM6" s="6">
+        <f t="shared" si="9"/>
+        <v>240.14285714285714</v>
+      </c>
+      <c r="BN6" s="6">
+        <f t="shared" si="9"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
@@ -5641,19 +5919,19 @@
       </c>
       <c r="Q7" s="16">
         <f>1.5*Q6</f>
-        <v>720</v>
+        <v>2880</v>
       </c>
       <c r="R7" s="17">
         <f t="shared" si="5"/>
-        <v>720</v>
+        <v>2880</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="6"/>
-        <v>0.20000016000000001</v>
+        <v>0.80000064000000004</v>
       </c>
       <c r="T7" s="5">
         <f t="shared" si="7"/>
-        <v>12.0000096</v>
+        <v>48.000038400000001</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>8</v>
@@ -5661,52 +5939,98 @@
       <c r="AL7" s="17">
         <v>10000</v>
       </c>
-      <c r="AM7" s="22">
+      <c r="AM7" s="16">
         <f t="shared" si="8"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AN7" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>204</v>
       </c>
       <c r="AO7" s="16">
-        <f t="shared" si="10"/>
-        <v>250.94897427831782</v>
+        <f t="shared" si="8"/>
+        <v>290.84271247461902</v>
       </c>
       <c r="AP7" s="16">
-        <f t="shared" si="11"/>
-        <v>290.84271247461902</v>
+        <f t="shared" si="8"/>
+        <v>416</v>
       </c>
       <c r="AQ7" s="16">
-        <f>MIN($AL7,AQ$1)+SQRT($AL7*AQ$1)</f>
+        <f t="shared" si="8"/>
         <v>1831.1388300841897</v>
       </c>
       <c r="AR7" s="16">
-        <f>MIN($AL7,AR$1)+SQRT($AL7*AR$1)</f>
+        <f t="shared" si="8"/>
         <v>20000</v>
       </c>
       <c r="AS7" s="16"/>
       <c r="AT7" s="16"/>
       <c r="AU7" s="16"/>
-      <c r="AW7" s="1" t="s">
+      <c r="AW7" s="1">
+        <f t="shared" si="10"/>
+        <v>10000000</v>
+      </c>
+      <c r="AX7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AX7" s="16">
+      <c r="AY7" s="16">
         <f t="shared" si="2"/>
         <v>127153.02220599999</v>
       </c>
-      <c r="AY7" s="16">
+      <c r="AZ7" s="16">
         <f>600000+2868750</f>
         <v>3468750</v>
       </c>
-      <c r="AZ7" s="16">
+      <c r="BA7" s="16">
         <v>113549713200</v>
       </c>
-      <c r="BA7" s="16">
+      <c r="BB7" s="16">
         <v>13599840256</v>
       </c>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD7" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="BE7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF7" s="6">
+        <f>2*BF6</f>
+        <v>96</v>
+      </c>
+      <c r="BG7" s="1">
+        <f t="shared" si="9"/>
+        <v>9025</v>
+      </c>
+      <c r="BH7" s="1">
+        <f t="shared" si="9"/>
+        <v>2116</v>
+      </c>
+      <c r="BI7" s="1">
+        <f t="shared" si="9"/>
+        <v>2883</v>
+      </c>
+      <c r="BJ7" s="6">
+        <f t="shared" si="9"/>
+        <v>2116</v>
+      </c>
+      <c r="BK7" s="6">
+        <f t="shared" si="9"/>
+        <v>1656.2</v>
+      </c>
+      <c r="BL7" s="6">
+        <f t="shared" si="9"/>
+        <v>1350</v>
+      </c>
+      <c r="BM7" s="6">
+        <f t="shared" si="9"/>
+        <v>1131.5714285714287</v>
+      </c>
+      <c r="BN7" s="6">
+        <f t="shared" si="9"/>
+        <v>968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -5725,11 +6049,11 @@
       </c>
       <c r="F8" s="16">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="3"/>
-        <v>44.729833462074168</v>
+        <v>52.721359549995796</v>
       </c>
       <c r="H8" s="16">
         <v>15.668749999999999</v>
@@ -5744,7 +6068,7 @@
       <c r="L8" s="16">
         <v>65000</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="27">
         <v>0.1</v>
       </c>
       <c r="N8" s="16">
@@ -5756,19 +6080,19 @@
       </c>
       <c r="Q8" s="16">
         <f>1.5*Q7</f>
-        <v>1080</v>
+        <v>4320</v>
       </c>
       <c r="R8" s="17">
         <f t="shared" si="5"/>
-        <v>1080</v>
+        <v>4320</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="6"/>
-        <v>0.30000024000000003</v>
+        <v>1.2000009600000001</v>
       </c>
       <c r="T8" s="5">
         <f t="shared" si="7"/>
-        <v>18.000014400000001</v>
+        <v>72.000057600000005</v>
       </c>
       <c r="V8" s="1">
         <f>1/3600</f>
@@ -5779,36 +6103,40 @@
       </c>
       <c r="AM8" s="16">
         <f t="shared" si="8"/>
-        <v>255.95097567963924</v>
+        <v>100</v>
       </c>
       <c r="AN8" s="16">
-        <f t="shared" si="9"/>
-        <v>513.90195135927843</v>
+        <f t="shared" si="8"/>
+        <v>400</v>
       </c>
       <c r="AO8" s="16">
-        <f t="shared" si="10"/>
-        <v>630.49979983983985</v>
+        <f t="shared" si="8"/>
+        <v>729.11025509279784</v>
       </c>
       <c r="AP8" s="16">
-        <f t="shared" si="11"/>
-        <v>729.11025509279784</v>
+        <f t="shared" si="8"/>
+        <v>1035.8039027185569</v>
       </c>
       <c r="AQ8" s="16">
-        <f>MIN($AL8,AQ$1)+SQRT($AL8*AQ$1)</f>
+        <f t="shared" si="8"/>
         <v>4281.1288741492754</v>
       </c>
-      <c r="AR8" s="23">
-        <f>MIN($AL8,AR$1)+SQRT($AL8*AR$1)</f>
+      <c r="AR8" s="16">
+        <f t="shared" si="8"/>
         <v>35495.097567963923</v>
       </c>
       <c r="AS8" s="16">
-        <f>MIN($AL8,AS$1)+SQRT($AL8*AS$1)</f>
+        <f t="shared" si="8"/>
         <v>130000</v>
       </c>
       <c r="AT8" s="16"/>
       <c r="AU8" s="16"/>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AW8" s="1">
+        <f t="shared" si="10"/>
+        <v>65000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -5827,11 +6155,11 @@
       </c>
       <c r="F9" s="16">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="3"/>
-        <v>250.94897427831782</v>
+        <v>290.84271247461902</v>
       </c>
       <c r="H9" s="16">
         <v>50.528750000000002</v>
@@ -5846,7 +6174,7 @@
       <c r="L9" s="16">
         <v>575000</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="28">
         <v>0.01</v>
       </c>
       <c r="N9" s="16">
@@ -5858,58 +6186,62 @@
       </c>
       <c r="Q9" s="16">
         <f>1.5*Q8</f>
-        <v>1620</v>
+        <v>6480</v>
       </c>
       <c r="R9" s="17">
         <f t="shared" si="5"/>
-        <v>1620</v>
+        <v>6480</v>
       </c>
       <c r="S9" s="4">
         <f t="shared" si="6"/>
-        <v>0.45000035999999999</v>
+        <v>1.80000144</v>
       </c>
       <c r="T9" s="5">
         <f t="shared" si="7"/>
-        <v>27.0000216</v>
+        <v>108.0000864</v>
       </c>
       <c r="AL9" s="17">
         <v>575000</v>
       </c>
       <c r="AM9" s="16">
         <f t="shared" si="8"/>
-        <v>759.28754440515502</v>
+        <v>100</v>
       </c>
       <c r="AN9" s="16">
-        <f t="shared" si="9"/>
-        <v>1520.57508881031</v>
+        <f t="shared" si="8"/>
+        <v>400</v>
       </c>
       <c r="AO9" s="16">
+        <f t="shared" si="8"/>
+        <v>2152.7610589527217</v>
+      </c>
+      <c r="AP9" s="16">
+        <f t="shared" si="8"/>
+        <v>3049.1501776206201</v>
+      </c>
+      <c r="AQ9" s="16">
+        <f t="shared" si="8"/>
+        <v>12239.578808281798</v>
+      </c>
+      <c r="AR9" s="16">
+        <f t="shared" si="8"/>
+        <v>85828.754440515506</v>
+      </c>
+      <c r="AS9" s="16">
+        <f t="shared" si="8"/>
+        <v>258326.14929181203</v>
+      </c>
+      <c r="AT9" s="16">
+        <f t="shared" si="8"/>
+        <v>1150000</v>
+      </c>
+      <c r="AU9" s="16"/>
+      <c r="AW9" s="1">
         <f t="shared" si="10"/>
-        <v>1863.4175621006709</v>
-      </c>
-      <c r="AP9" s="16">
-        <f t="shared" si="11"/>
-        <v>2152.7610589527217</v>
-      </c>
-      <c r="AQ9" s="16">
-        <f>MIN($AL9,AQ$1)+SQRT($AL9*AQ$1)</f>
-        <v>12239.578808281798</v>
-      </c>
-      <c r="AR9" s="27">
-        <f>MIN($AL9,AR$1)+SQRT($AL9*AR$1)</f>
-        <v>85828.754440515506</v>
-      </c>
-      <c r="AS9" s="16">
-        <f>MIN($AL9,AS$1)+SQRT($AL9*AS$1)</f>
-        <v>258326.14929181203</v>
-      </c>
-      <c r="AT9" s="16">
-        <f>MIN($AL9,AT$1)+SQRT($AL9*AT$1)</f>
-        <v>1150000</v>
-      </c>
-      <c r="AU9" s="16"/>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+        <v>575000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>85</v>
       </c>
@@ -5947,48 +6279,52 @@
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
-      <c r="R10" s="30"/>
+      <c r="R10" s="26"/>
       <c r="AL10" s="17">
         <v>1000000</v>
       </c>
       <c r="AM10" s="16">
         <f t="shared" si="8"/>
-        <v>1001</v>
+        <v>100</v>
       </c>
       <c r="AN10" s="16">
-        <f t="shared" si="9"/>
-        <v>2004</v>
+        <f t="shared" si="8"/>
+        <v>400</v>
       </c>
       <c r="AO10" s="16">
+        <f t="shared" si="8"/>
+        <v>2836.4271247461902</v>
+      </c>
+      <c r="AP10" s="16">
+        <f t="shared" si="8"/>
+        <v>4016</v>
+      </c>
+      <c r="AQ10" s="16">
+        <f t="shared" si="8"/>
+        <v>16061.388300841896</v>
+      </c>
+      <c r="AR10" s="16">
+        <f t="shared" si="8"/>
+        <v>110000</v>
+      </c>
+      <c r="AS10" s="16">
+        <f t="shared" si="8"/>
+        <v>319950.97567963926</v>
+      </c>
+      <c r="AT10" s="16">
+        <f t="shared" si="8"/>
+        <v>1333287.5444051549</v>
+      </c>
+      <c r="AU10" s="16">
+        <f>MIN(AU$12,$AW10,MIN($AL10,AU$1)+SQRT($AL10*AU$1))</f>
+        <v>2000000</v>
+      </c>
+      <c r="AW10" s="1">
         <f t="shared" si="10"/>
-        <v>2455.4897427831779</v>
-      </c>
-      <c r="AP10" s="16">
-        <f t="shared" si="11"/>
-        <v>2836.4271247461902</v>
-      </c>
-      <c r="AQ10" s="16">
-        <f>MIN($AL10,AQ$1)+SQRT($AL10*AQ$1)</f>
-        <v>16061.388300841896</v>
-      </c>
-      <c r="AR10" s="16">
-        <f>MIN($AL10,AR$1)+SQRT($AL10*AR$1)</f>
-        <v>110000</v>
-      </c>
-      <c r="AS10" s="16">
-        <f>MIN($AL10,AS$1)+SQRT($AL10*AS$1)</f>
-        <v>319950.97567963926</v>
-      </c>
-      <c r="AT10" s="16">
-        <f>MIN($AL10,AT$1)+SQRT($AL10*AT$1)</f>
-        <v>1333287.5444051549</v>
-      </c>
-      <c r="AU10" s="16">
-        <f>MIN($AL10,AU$1)+SQRT($AL10*AU$1)</f>
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -6033,7 +6369,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -6068,8 +6404,44 @@
       <c r="R12" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AM12" s="1">
+        <f>AW2</f>
+        <v>100</v>
+      </c>
+      <c r="AN12" s="1">
+        <f>AW3</f>
+        <v>400</v>
+      </c>
+      <c r="AO12" s="1">
+        <f>AW4</f>
+        <v>8000</v>
+      </c>
+      <c r="AP12" s="1">
+        <f>AW5</f>
+        <v>16000</v>
+      </c>
+      <c r="AQ12" s="1">
+        <f>AW6</f>
+        <v>250000</v>
+      </c>
+      <c r="AR12" s="1">
+        <f>AW7</f>
+        <v>10000000</v>
+      </c>
+      <c r="AS12" s="1">
+        <f>AW8</f>
+        <v>65000000</v>
+      </c>
+      <c r="AT12" s="1">
+        <f>AW9</f>
+        <v>575000000</v>
+      </c>
+      <c r="AU12" s="1">
+        <f>AW10</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
@@ -6084,7 +6456,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>4.51</v>
       </c>
@@ -6095,7 +6467,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="Q14" s="33">
+      <c r="Q14" s="29">
         <v>0.01</v>
       </c>
       <c r="R14" s="1">
@@ -6105,8 +6477,11 @@
         <f>R14*TAN(RADIANS(Q$14))</f>
         <v>6.9813170788650121E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AK14" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f>B14*3600</f>
         <v>16236</v>
@@ -6123,7 +6498,7 @@
       </c>
       <c r="G15" s="1">
         <f>2*R5</f>
-        <v>640</v>
+        <v>2560</v>
       </c>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -6133,11 +6508,14 @@
         <v>16</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" ref="S15:S21" si="12">R15*TAN(RADIANS(Q$14))</f>
+        <f t="shared" ref="S15:S21" si="11">R15*TAN(RADIANS(Q$14))</f>
         <v>2.7925268315460048E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AK15" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>120</v>
       </c>
@@ -6147,7 +6525,7 @@
       </c>
       <c r="G16" s="1">
         <f>2*R6</f>
-        <v>960</v>
+        <v>3840</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -6157,11 +6535,14 @@
         <v>50</v>
       </c>
       <c r="S16" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>8.7266463485812656E-3</v>
       </c>
-    </row>
-    <row r="17" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AK16" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>7.5</v>
       </c>
@@ -6177,7 +6558,7 @@
       </c>
       <c r="G17" s="1">
         <f>2*R7</f>
-        <v>1440</v>
+        <v>5760</v>
       </c>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
@@ -6187,11 +6568,14 @@
         <v>90</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1.5707963427446278E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AK17" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <f>60*B17</f>
         <v>450</v>
@@ -6201,7 +6585,7 @@
       </c>
       <c r="G18" s="1">
         <f>SUM(G15:G17)</f>
-        <v>3040</v>
+        <v>12160</v>
       </c>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
@@ -6211,17 +6595,20 @@
         <v>20000</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.490658539432506</v>
       </c>
-    </row>
-    <row r="19" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AK18" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="F19" s="1" t="s">
         <v>121</v>
       </c>
       <c r="G19" s="1">
         <f>G18+450</f>
-        <v>3490</v>
+        <v>12610</v>
       </c>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -6231,17 +6618,20 @@
         <v>36000</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>6.2831853709785106</v>
       </c>
-    </row>
-    <row r="20" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AK19" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="F20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="4">
         <f>G19/3600</f>
-        <v>0.96944444444444444</v>
+        <v>3.5027777777777778</v>
       </c>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
@@ -6251,53 +6641,540 @@
         <v>86000</v>
       </c>
       <c r="S20" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>15.009831719559775</v>
       </c>
-    </row>
-    <row r="21" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AK20" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="R21" s="1">
         <v>128000</v>
       </c>
       <c r="S21" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>22.34021465236804</v>
       </c>
-    </row>
-    <row r="22" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AK21" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="S22" s="5"/>
     </row>
-    <row r="23" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E23" s="5">
+        <f>2.86875-0.6+1.2</f>
+        <v>3.46875</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <f>INDEX($N$23:$N$31,F23)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1">
+        <f>INDEX($N$23:$N$31,H23)</f>
+        <v>5</v>
+      </c>
+      <c r="J23" s="6">
+        <f>MIN(G23+I23)+SQRT(G23*I23)</f>
+        <v>8.2360679774997898</v>
+      </c>
+      <c r="K23" s="36" t="str">
+        <f>IF(J23&gt;=E23,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="S23" s="5"/>
       <c r="AJ23" s="16"/>
       <c r="AK23" s="16"/>
     </row>
-    <row r="24" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E24" s="5">
+        <f>2.86875*2+0.6*2</f>
+        <v>6.9375</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <f>INDEX($N$23:$N$31,F24)</f>
+        <v>5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1">
+        <f>INDEX($N$23:$N$31,H24)</f>
+        <v>5</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" ref="J24:J31" si="12">MIN(G24+I24)+SQRT(G24*I24)</f>
+        <v>15</v>
+      </c>
+      <c r="K24" s="36" t="str">
+        <f>IF(J24&gt;=E24,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M24" s="1">
+        <f>1+M23</f>
+        <v>2</v>
+      </c>
+      <c r="N24" s="1">
+        <v>5</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="P24" s="1">
+        <f>N24/N23</f>
+        <v>5</v>
+      </c>
       <c r="S24" s="5"/>
     </row>
-    <row r="25" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E25" s="1">
+        <f>12+0.3-0.6+1</f>
+        <v>12.700000000000001</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <f>INDEX($N$23:$N$31,F25)</f>
+        <v>5</v>
+      </c>
+      <c r="H25" s="2">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1">
+        <f>INDEX($N$23:$N$31,H25)</f>
+        <v>35</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="12"/>
+        <v>53.228756555322953</v>
+      </c>
+      <c r="K25" s="36" t="str">
+        <f>IF(J25&gt;=E25,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" ref="M25:M31" si="13">1+M24</f>
+        <v>3</v>
+      </c>
+      <c r="N25" s="1">
+        <v>35</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="P25" s="1">
+        <f>N25/N24</f>
+        <v>7</v>
+      </c>
       <c r="S25" s="5"/>
     </row>
-    <row r="26" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" s="1">
+        <f>47+0.2-0.6+1</f>
+        <v>47.6</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <f>INDEX($N$23:$N$31,F26)</f>
+        <v>5</v>
+      </c>
+      <c r="H26" s="2">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1">
+        <f>INDEX($N$23:$N$31,H26)</f>
+        <v>35</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="12"/>
+        <v>53.228756555322953</v>
+      </c>
+      <c r="K26" s="36" t="str">
+        <f>IF(J26&gt;=E26,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="N26" s="1">
+        <f>5*N25</f>
+        <v>175</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="P26" s="1">
+        <f>N26/N25</f>
+        <v>5</v>
+      </c>
       <c r="S26" s="5"/>
     </row>
-    <row r="27" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E27" s="1">
+        <v>85</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <f>INDEX($N$23:$N$31,F27)</f>
+        <v>5</v>
+      </c>
+      <c r="H27" s="2">
+        <v>4</v>
+      </c>
+      <c r="I27" s="1">
+        <f>INDEX($N$23:$N$31,H27)</f>
+        <v>175</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="12"/>
+        <v>209.58039891549808</v>
+      </c>
+      <c r="K27" s="36" t="str">
+        <f>IF(J27&gt;=E27,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="N27" s="1">
+        <v>20000</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="P27" s="1">
+        <f>N27/N26</f>
+        <v>114.28571428571429</v>
+      </c>
       <c r="S27" s="5"/>
     </row>
-    <row r="28" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E28" s="1">
+        <v>19000</v>
+      </c>
+      <c r="F28" s="2">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <f>INDEX($N$23:$N$31,F28)</f>
+        <v>35</v>
+      </c>
+      <c r="H28" s="2">
+        <v>5</v>
+      </c>
+      <c r="I28" s="1">
+        <f>INDEX($N$23:$N$31,H28)</f>
+        <v>20000</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="12"/>
+        <v>20871.660026534075</v>
+      </c>
+      <c r="K28" s="36" t="str">
+        <f>IF(J28&gt;=E28,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" ref="N26:N31" si="14">4*N27</f>
+        <v>80000</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="P28" s="1">
+        <f>N28/N27</f>
+        <v>4</v>
+      </c>
       <c r="S28" s="5"/>
     </row>
-    <row r="29" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E29" s="1">
+        <v>36000</v>
+      </c>
+      <c r="F29" s="2">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <f>INDEX($N$23:$N$31,F29)</f>
+        <v>35</v>
+      </c>
+      <c r="H29" s="2">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1">
+        <f>INDEX($N$23:$N$31,H29)</f>
+        <v>80000</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="12"/>
+        <v>81708.32005306815</v>
+      </c>
+      <c r="K29" s="36" t="str">
+        <f>IF(J29&gt;=E29,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M29" s="1">
+        <v>7</v>
+      </c>
+      <c r="N29" s="1">
+        <v>160000</v>
+      </c>
+      <c r="P29" s="1">
+        <f>N29/N28</f>
+        <v>2</v>
+      </c>
       <c r="S29" s="5"/>
     </row>
-    <row r="30" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E30" s="1">
+        <v>86000</v>
+      </c>
+      <c r="F30" s="2">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <f>INDEX($N$23:$N$31,F30)</f>
+        <v>175</v>
+      </c>
+      <c r="H30" s="2">
+        <v>7</v>
+      </c>
+      <c r="I30" s="1">
+        <f>INDEX($N$23:$N$31,H30)</f>
+        <v>160000</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="12"/>
+        <v>165466.50262212919</v>
+      </c>
+      <c r="K30" s="36" t="str">
+        <f>IF(J30&gt;=E30,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="M30" s="1">
+        <v>8</v>
+      </c>
+      <c r="N30" s="1">
+        <v>320000</v>
+      </c>
+      <c r="P30" s="1">
+        <f>N30/N29</f>
+        <v>2</v>
+      </c>
       <c r="S30" s="5"/>
     </row>
-    <row r="31" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E31" s="1">
+        <v>186000</v>
+      </c>
+      <c r="F31" s="2">
+        <v>4</v>
+      </c>
+      <c r="G31" s="1">
+        <f>INDEX($N$23:$N$31,F31)</f>
+        <v>175</v>
+      </c>
+      <c r="H31" s="2">
+        <v>8</v>
+      </c>
+      <c r="I31" s="1">
+        <f>INDEX($N$23:$N$31,H31)</f>
+        <v>320000</v>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="12"/>
+        <v>327658.31477354787</v>
+      </c>
+      <c r="K31" s="36" t="str">
+        <f>IF(J31&gt;=E31,"yes","no")</f>
+        <v>yes</v>
+      </c>
       <c r="S31" s="5"/>
       <c r="AL31" s="16"/>
     </row>
-    <row r="32" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="S32" s="5"/>
       <c r="AL32" s="16"/>
     </row>
@@ -6318,6 +7195,7 @@
     <sortCondition ref="AL23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6510,13 +7388,13 @@
         <f>2*PI()*SQRT(H3^3/I3)</f>
         <v>1833.6072536492711</v>
       </c>
-      <c r="R3" s="41">
+      <c r="R3" s="37">
         <v>2223</v>
       </c>
-      <c r="S3" s="41">
+      <c r="S3" s="37">
         <v>71</v>
       </c>
-      <c r="T3" s="41">
+      <c r="T3" s="37">
         <v>10</v>
       </c>
     </row>
@@ -6710,7 +7588,7 @@
         <f>2*PI()*SQRT(H7^3/I7)</f>
         <v>53310.658020675924</v>
       </c>
-      <c r="R7" s="39">
+      <c r="R7" s="35">
         <f>T3*S3^2</f>
         <v>50410</v>
       </c>
@@ -7080,34 +7958,34 @@
       <c r="C2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="25">
         <v>0.6</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="25">
         <f t="shared" ref="E2:K2" si="0">5%+D2</f>
         <v>0.65</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="25">
         <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="25">
         <f t="shared" si="0"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" s="25">
         <f t="shared" si="0"/>
         <v>0.80000000000000016</v>
       </c>
-      <c r="I2" s="29">
+      <c r="I2" s="25">
         <f t="shared" si="0"/>
         <v>0.8500000000000002</v>
       </c>
-      <c r="J2" s="29">
+      <c r="J2" s="25">
         <f t="shared" si="0"/>
         <v>0.90000000000000024</v>
       </c>
-      <c r="K2" s="29">
+      <c r="K2" s="25">
         <f t="shared" si="0"/>
         <v>0.95000000000000029</v>
       </c>
@@ -7196,34 +8074,34 @@
       <c r="G6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="25">
         <v>0.6</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="25">
         <f t="shared" ref="I6:O6" si="2">5%+H6</f>
         <v>0.65</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="25">
         <f t="shared" si="2"/>
         <v>0.70000000000000007</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="25">
         <f t="shared" si="2"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="25">
         <f t="shared" si="2"/>
         <v>0.80000000000000016</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="25">
         <f t="shared" si="2"/>
         <v>0.8500000000000002</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N6" s="25">
         <f t="shared" si="2"/>
         <v>0.90000000000000024</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="25">
         <f t="shared" si="2"/>
         <v>0.95000000000000029</v>
       </c>
@@ -7364,47 +8242,47 @@
       <c r="D10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>0.6</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="25">
         <f>5%+E10</f>
         <v>0.65</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="25">
         <f>5%+F10</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="25">
         <f>5%+G10</f>
         <v>0.75000000000000011</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="25">
         <f>5%+H10</f>
         <v>0.80000000000000016</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="25">
         <f>5%+I10</f>
         <v>0.8500000000000002</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="25">
         <v>0.87</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="25">
         <f>5%+J10</f>
         <v>0.90000000000000024</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="25">
         <v>0.92</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="25">
         <f>5%+L10</f>
         <v>0.95000000000000029</v>
       </c>
       <c r="P10" s="1">
         <v>2.5</v>
       </c>
-      <c r="Q10" s="35">
+      <c r="Q10" s="31">
         <f>P10/P11*Q11</f>
         <v>4.3679066666666664</v>
       </c>
@@ -7534,7 +8412,7 @@
       <c r="A13" s="2">
         <v>1.25</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="38">
         <v>0.5</v>
       </c>
       <c r="C13" s="1">
@@ -7593,7 +8471,7 @@
       <c r="A14" s="2">
         <v>2.5</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14" s="38">
         <v>1.8</v>
       </c>
       <c r="C14" s="1">
@@ -7653,7 +8531,7 @@
       <c r="A15" s="2">
         <v>2.5</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15" s="38">
         <v>6</v>
       </c>
       <c r="C15" s="1">
@@ -7709,7 +8587,7 @@
       <c r="A16" s="2">
         <v>2.5</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16" s="38">
         <v>2</v>
       </c>
       <c r="C16" s="1">
@@ -7768,7 +8646,7 @@
       <c r="A17" s="2">
         <v>2.5</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="38">
         <v>2.4</v>
       </c>
       <c r="C17" s="1">
@@ -7828,7 +8706,7 @@
       <c r="A18" s="2">
         <v>3.75</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18" s="38">
         <v>3.5</v>
       </c>
       <c r="C18" s="1">
@@ -7884,7 +8762,7 @@
       <c r="A19" s="2">
         <v>2.5</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19" s="38">
         <v>1.9</v>
       </c>
       <c r="C19" s="1">
@@ -7940,7 +8818,7 @@
       <c r="A20" s="2">
         <v>2.5</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="38">
         <v>4.5999999999999996</v>
       </c>
       <c r="C20" s="1">
@@ -7996,7 +8874,7 @@
       <c r="A21" s="2">
         <v>3.75</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="38">
         <v>6</v>
       </c>
       <c r="C21" s="1">
@@ -8052,7 +8930,7 @@
       <c r="A22" s="2">
         <v>1.875</v>
       </c>
-      <c r="B22" s="42">
+      <c r="B22" s="38">
         <v>3.5</v>
       </c>
       <c r="C22" s="1">
@@ -8160,40 +9038,40 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="39">
+      <c r="B2" s="35">
         <v>5</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="35">
         <f>60*B2</f>
         <v>300</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="35">
         <f>250*B2</f>
         <v>1250</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="39">
+      <c r="B3" s="35">
         <v>8</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="35">
         <f>60*B3</f>
         <v>480</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="35">
         <f>250*B3</f>
         <v>2000</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="39">
+      <c r="B4" s="35">
         <v>0.5</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="35">
         <f>60*B4</f>
         <v>30</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="35">
         <f>250*B4</f>
         <v>125</v>
       </c>
@@ -8217,7 +9095,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>198</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -8231,10 +9109,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="1">
         <v>1.25</v>
       </c>
@@ -8242,10 +9120,10 @@
         <f>2*PI()*C2/2*C3</f>
         <v>4.908738521234052</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="1">
         <v>0.54</v>
       </c>
@@ -8255,17 +9133,17 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="1">
         <v>1.25</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="1">
         <v>0.26</v>
       </c>
@@ -8275,10 +9153,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="1">
         <v>3.7499999999999999E-3</v>
       </c>
@@ -8286,19 +9164,19 @@
         <f>C4*D2</f>
         <v>1.8407769454627694E-2</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="1">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="1">
         <v>0.6</v>
       </c>
@@ -8308,27 +9186,27 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="40">
         <f>D5/2</f>
         <v>5.5223308363883082E-3</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="30" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="F7" s="34" t="s">
+      <c r="B7" s="30"/>
+      <c r="F7" s="30" t="s">
         <v>177</v>
       </c>
       <c r="H7" s="1">
@@ -8344,11 +9222,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="F8" s="34" t="s">
+      <c r="B8" s="30"/>
+      <c r="F8" s="30" t="s">
         <v>178</v>
       </c>
       <c r="H8" s="1">
@@ -8364,11 +9242,11 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="F9" s="34" t="s">
+      <c r="B9" s="30"/>
+      <c r="F9" s="30" t="s">
         <v>179</v>
       </c>
       <c r="H9" s="1">
@@ -8380,11 +9258,11 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="F10" s="34" t="s">
+      <c r="B10" s="30"/>
+      <c r="F10" s="30" t="s">
         <v>183</v>
       </c>
       <c r="H10" s="1">
@@ -8400,25 +9278,25 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="F11" s="34" t="s">
+      <c r="B11" s="30"/>
+      <c r="F11" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="35">
         <f>I10*H9*H10*PI()/3</f>
         <v>6.5143050792210236E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="30" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="30" t="s">
         <v>173</v>
       </c>
       <c r="C13" s="1">
@@ -8428,12 +9306,12 @@
         <f>2*PI()*C13/2*C14</f>
         <v>98.174770424681029</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="30" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="30" t="s">
         <v>174</v>
       </c>
       <c r="C14" s="1">
@@ -8443,23 +9321,23 @@
         <f>C15*D13</f>
         <v>1.4726215563702154</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="30" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C15" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="30" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="30" t="s">
         <v>194</v>
       </c>
       <c r="C16" s="1">
@@ -8469,29 +9347,29 @@
         <f>C16*D14</f>
         <v>0.8835729338221292</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="30" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="30" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="40">
         <f>D16/2</f>
         <v>0.4417864669110646</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="30" t="s">
         <v>205</v>
       </c>
       <c r="C20" s="1">
@@ -8503,7 +9381,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="30" t="s">
         <v>206</v>
       </c>
       <c r="C21" s="1">
@@ -8515,7 +9393,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="30" t="s">
         <v>175</v>
       </c>
       <c r="C22" s="1">
@@ -8523,7 +9401,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="30" t="s">
         <v>194</v>
       </c>
       <c r="C23" s="1">
@@ -8531,7 +9409,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="30" t="s">
         <v>207</v>
       </c>
       <c r="C24" s="1">
@@ -8539,17 +9417,17 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="30" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="30" t="s">
         <v>169</v>
       </c>
       <c r="C28" s="1">
@@ -8569,7 +9447,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="30" t="s">
         <v>170</v>
       </c>
       <c r="C29" s="1">
@@ -8591,7 +9469,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="30" t="s">
         <v>171</v>
       </c>
       <c r="C30" s="1">
@@ -8615,7 +9493,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="30" t="s">
         <v>172</v>
       </c>
       <c r="C31" s="1">
@@ -8639,7 +9517,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="30" t="s">
         <v>208</v>
       </c>
       <c r="C32" s="1">
@@ -8663,7 +9541,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="30" t="s">
         <v>209</v>
       </c>
       <c r="D33" s="1">
@@ -8684,7 +9562,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="30" t="s">
         <v>210</v>
       </c>
       <c r="D34" s="1">
@@ -8705,7 +9583,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="30" t="s">
         <v>211</v>
       </c>
       <c r="D35" s="1">
@@ -8726,7 +9604,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="30" t="s">
         <v>212</v>
       </c>
       <c r="D36" s="1">
@@ -8747,12 +9625,12 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="30" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="30" t="s">
         <v>214</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -8760,7 +9638,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="30" t="s">
         <v>215</v>
       </c>
       <c r="E39" s="1">
@@ -8769,7 +9647,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="30" t="s">
         <v>216</v>
       </c>
       <c r="E40" s="1">
@@ -8778,7 +9656,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="30" t="s">
         <v>217</v>
       </c>
       <c r="E41" s="1">
@@ -8787,7 +9665,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="30" t="s">
         <v>218</v>
       </c>
       <c r="E42" s="1">
@@ -8796,7 +9674,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="30" t="s">
         <v>219</v>
       </c>
       <c r="E43" s="1">
@@ -8805,12 +9683,12 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="30" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="30" t="s">
         <v>222</v>
       </c>
       <c r="C46" s="1">
@@ -8830,7 +9708,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="30" t="s">
         <v>223</v>
       </c>
       <c r="C47" s="1">
@@ -8853,7 +9731,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="30" t="s">
         <v>224</v>
       </c>
       <c r="C48" s="1">
@@ -8877,7 +9755,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="30" t="s">
         <v>172</v>
       </c>
       <c r="C49" s="1">
@@ -8901,7 +9779,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="30" t="s">
         <v>225</v>
       </c>
       <c r="C50" s="1">
@@ -8925,7 +9803,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="30" t="s">
         <v>226</v>
       </c>
       <c r="D51" s="1">
@@ -8946,7 +9824,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="30" t="s">
         <v>227</v>
       </c>
       <c r="D52" s="1">
@@ -8967,7 +9845,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="30" t="s">
         <v>228</v>
       </c>
       <c r="D53" s="1">
@@ -8988,7 +9866,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="30" t="s">
         <v>229</v>
       </c>
       <c r="D54" s="1">
@@ -9009,42 +9887,42 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="30" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="30" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="30" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="34" t="s">
+      <c r="A59" s="30" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="34" t="s">
+      <c r="A60" s="30" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="34" t="s">
+      <c r="A61" s="30" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="30" t="s">
         <v>237</v>
       </c>
     </row>
@@ -9057,8 +9935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9067,10 +9945,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>277</v>
       </c>
     </row>
@@ -9101,8 +9979,8 @@
         <f>C2^2+C2*C3+C3^2</f>
         <v>0.68359375</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -9123,16 +10001,20 @@
       <c r="B5" s="1">
         <v>0.04</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="40">
         <f>D4*B5</f>
         <v>9.3061501131728903E-3</v>
       </c>
+      <c r="H5" s="1">
+        <f>0.1*0.2*0.28</f>
+        <v>5.6000000000000017E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>277</v>
       </c>
     </row>
@@ -9183,13 +10065,13 @@
       <c r="B11" s="1">
         <v>0.04</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="40">
         <f>D10*B11</f>
         <v>1.3892960472215024</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="30" t="s">
         <v>279</v>
       </c>
     </row>
@@ -9204,6 +10086,7 @@
         <f>B14/2</f>
         <v>0.75</v>
       </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -9240,7 +10123,7 @@
       <c r="B17" s="1">
         <v>0.04</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="40">
         <f>D16*B17</f>
         <v>9.6211275016187411E-2</v>
       </c>
@@ -9288,7 +10171,7 @@
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="44">
+      <c r="B25" s="40">
         <f>0.000007*B24</f>
         <v>5.3474570265693452E-2</v>
       </c>
@@ -9314,10 +10197,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="41" t="s">
         <v>260</v>
       </c>
     </row>
@@ -9604,7 +10487,7 @@
       <c r="L9" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="31">
         <f>AVERAGE(M3,M5,M6)</f>
         <v>1.3771710530963608E-2</v>
       </c>
@@ -9704,10 +10587,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="41" t="s">
         <v>259</v>
       </c>
       <c r="F16" s="13"/>
@@ -9973,13 +10856,13 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="41" t="s">
         <v>267</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="41" t="s">
         <v>268</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="30" t="s">
         <v>279</v>
       </c>
     </row>
@@ -10028,7 +10911,7 @@
         <f>B27/2</f>
         <v>0.79800000000000004</v>
       </c>
-      <c r="D27" s="35">
+      <c r="D27" s="31">
         <f>PI()*(C26+C27)*SQRT((C26-C27)^2+B28^2)</f>
         <v>2.0781234452196751</v>
       </c>
@@ -10042,7 +10925,7 @@
         <f>G27/2</f>
         <v>1.25</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I27" s="31">
         <f>PI()*(H26+H27)*SQRT((H26-H27)^2+G28^2)</f>
         <v>5.6635866995694881</v>
       </c>
@@ -10086,7 +10969,7 @@
       <c r="B29" s="1">
         <v>0.38100000000000001</v>
       </c>
-      <c r="D29" s="35">
+      <c r="D29" s="31">
         <f>2*PI()*C27*B29</f>
         <v>1.910327094424267</v>
       </c>
@@ -10159,7 +11042,7 @@
       <c r="B31" s="1">
         <v>67.7</v>
       </c>
-      <c r="D31" s="35">
+      <c r="D31" s="31">
         <f>D29*D27*B30</f>
         <v>9.9247388074036227E-2</v>
       </c>
@@ -10239,7 +11122,7 @@
         <f>B34/2</f>
         <v>0.79800000000000004</v>
       </c>
-      <c r="D34" s="35">
+      <c r="D34" s="31">
         <f>PI()*(C33+C34)*SQRT((C33-C34)^2+B35^2)</f>
         <v>2.0781234452196751</v>
       </c>
@@ -10289,7 +11172,7 @@
       <c r="B36" s="1">
         <v>0.73660000000000003</v>
       </c>
-      <c r="D36" s="35">
+      <c r="D36" s="31">
         <f>2*PI()*C34*B36</f>
         <v>3.6932990492202498</v>
       </c>
@@ -10318,7 +11201,7 @@
       <c r="B38" s="1">
         <v>114.4</v>
       </c>
-      <c r="D38" s="35">
+      <c r="D38" s="31">
         <f>D36*D34*B37</f>
         <v>0.19187828360980341</v>
       </c>

</xml_diff>